<commit_message>
Magic sheet Names moved to ExcelProperties class
</commit_message>
<xml_diff>
--- a/excelTemps/customers.xlsx
+++ b/excelTemps/customers.xlsx
@@ -12,10 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7815"/>
   </bookViews>
   <sheets>
-    <sheet name="REFERENCES" sheetId="1" r:id="rId1"/>
+    <sheet name="CUSTOMERS" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">REFERENCES!$A$2:$I$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CUSTOMERS!$A$2:$I$2</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -199,16 +199,16 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -497,7 +497,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,40 +511,40 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
+      <c r="A2" s="3"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
       <c r="I2" s="7"/>
     </row>
   </sheetData>

</xml_diff>